<commit_message>
Commit for new Branch
</commit_message>
<xml_diff>
--- a/sheet.XLSX
+++ b/sheet.XLSX
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>jb</t>
   </si>
@@ -52,6 +52,21 @@
   </si>
   <si>
     <t>gsdgf</t>
+  </si>
+  <si>
+    <t>wfwef</t>
+  </si>
+  <si>
+    <t>wfwfwef</t>
+  </si>
+  <si>
+    <t>wefwe</t>
+  </si>
+  <si>
+    <t>fwef</t>
+  </si>
+  <si>
+    <t>fwefwe</t>
   </si>
 </sst>
 </file>
@@ -390,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A16"/>
+  <dimension ref="A1:A21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,7 +485,32 @@
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>8</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>